<commit_message>
functie aanpassen_naar_gemiddeld gefixt en verbeterd
</commit_message>
<xml_diff>
--- a/omloop planning energie verbruik test.xlsx
+++ b/omloop planning energie verbruik test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VScode\busje-komt-zo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C6507E-7168-45FA-9577-6A6019D88D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB89AFF0-7A14-41FF-BC5F-6AD4D5302ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25680" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21510" yWindow="2355" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2367,7 +2367,7 @@
   <dimension ref="A1:K721"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2831,7 +2831,7 @@
         <v>14</v>
       </c>
       <c r="H14">
-        <v>10.32</v>
+        <v>1000.32</v>
       </c>
       <c r="I14" s="2">
         <v>45106.34097222222</v>
@@ -26436,6 +26436,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100931431478CF5164F9F4426B07FCEC3C0" ma:contentTypeVersion="12" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="04af3a1d4f66cf43f76c3176d0feadf6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dbd7ad12-3323-416c-89da-709eb039707f" xmlns:ns3="c4c90c3b-e0bd-4787-87d0-fc55f607185c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6b79c2f15acc46f6342802de4a071dd" ns2:_="" ns3:_="">
     <xsd:import namespace="dbd7ad12-3323-416c-89da-709eb039707f"/>
@@ -26646,16 +26655,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8C3BC0-E912-4338-A876-A3F97CCE5DE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7567438-8C04-4FBA-BDB9-3461D59EC70C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26672,12 +26680,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8C3BC0-E912-4338-A876-A3F97CCE5DE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>